<commit_message>
updated choosing arena and skybox in title
</commit_message>
<xml_diff>
--- a/TODO Spreadsheet.xlsx
+++ b/TODO Spreadsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>Transfer DODO txt document to Excel sheet</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>TItleScreen - fix camera</t>
+  </si>
+  <si>
+    <t>TODO: update controls/have controls blinking on bottom of screen or something</t>
+  </si>
+  <si>
+    <t>Fiddling</t>
+  </si>
+  <si>
+    <t>CarScreen - fix the "Player X…. " text so that doesn't switch when done</t>
+  </si>
+  <si>
+    <t>TitleScreen - "PLAY" button before going to start of game?</t>
+  </si>
+  <si>
+    <t>TitleScreen - fix colour of text, black sort of hard to see</t>
+  </si>
+  <si>
+    <t>Fix pause menu</t>
   </si>
 </sst>
 </file>
@@ -554,11 +572,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +919,7 @@
         <v>42933</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
@@ -909,7 +927,7 @@
         <v>42933</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>42</v>
       </c>
@@ -920,7 +938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>43</v>
       </c>
@@ -931,7 +949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>45</v>
       </c>
@@ -942,7 +960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>44</v>
       </c>
@@ -953,7 +971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>46</v>
       </c>
@@ -964,7 +982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>47</v>
       </c>
@@ -975,7 +993,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>48</v>
       </c>
@@ -989,7 +1007,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1000,7 +1018,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1011,7 +1029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>53</v>
       </c>
@@ -1022,36 +1040,86 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C44" s="1">
         <v>42940</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C45" s="1">
         <v>42940</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C46" s="1">
         <v>42940</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C47" s="1">
         <v>42940</v>
+      </c>
+      <c r="D47" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="1">
+        <v>42941</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="1">
+        <v>42941</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="1">
+        <v>42941</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Essentially done main parts of fixing title screen
</commit_message>
<xml_diff>
--- a/TODO Spreadsheet.xlsx
+++ b/TODO Spreadsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
   <si>
     <t>Transfer DODO txt document to Excel sheet</t>
   </si>
@@ -108,9 +108,6 @@
     <t>ETC Things</t>
   </si>
   <si>
-    <t>Put back to fullscreen once done</t>
-  </si>
-  <si>
     <t xml:space="preserve"> check if vehicle is human and only play sfx for human cars</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Make title screen code better -&gt;interfaces?</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Config file for variables</t>
   </si>
   <si>
@@ -171,12 +165,6 @@
     <t>TitleScreen.cpp - make better now that other Screens are done</t>
   </si>
   <si>
-    <t>Get textures showing up</t>
-  </si>
-  <si>
-    <t>Done positions</t>
-  </si>
-  <si>
     <t>Fix updateGameText</t>
   </si>
   <si>
@@ -207,7 +195,31 @@
     <t>TitleScreen - fix colour of text, black sort of hard to see</t>
   </si>
   <si>
-    <t>Fix pause menu</t>
+    <t>Fix pause menu-update it</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Decided against; did something different</t>
+  </si>
+  <si>
+    <t>Date Completed</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Still messing around with variables, but main part done</t>
+  </si>
+  <si>
+    <t>Main parts done, just fiddling</t>
+  </si>
+  <si>
+    <t>Don't need anymore</t>
   </si>
 </sst>
 </file>
@@ -572,23 +584,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="53.5546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
@@ -598,59 +613,80 @@
       <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="F1" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>42903</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>42903</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>42903</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>42903</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>42903</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>42903</v>
@@ -658,473 +694,607 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
-        <v>42903</v>
+        <v>42904</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
-        <v>42903</v>
+        <v>42904</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>42903</v>
+        <v>42904</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>42903</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42921</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
-        <v>42903</v>
+        <v>42921</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1">
-        <v>42904</v>
+        <v>42923</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
-        <v>42904</v>
+        <v>42924</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1">
-        <v>42904</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42928</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1">
-        <v>42904</v>
+        <v>42924</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>42921</v>
+        <v>42927</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1">
-        <v>42921</v>
+        <v>42928</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1">
-        <v>42923</v>
+        <v>42928</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42935</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="1">
+        <v>42935</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1">
+        <v>42935</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="1">
+        <v>42935</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1">
+        <v>42935</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1">
+        <v>42935</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="1">
+        <v>42938</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1">
+        <v>42940</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1">
+        <v>42940</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="1">
+        <v>42940</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1">
+        <v>42940</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="1">
+        <v>42938</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C32" s="1">
         <v>42924</v>
       </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1">
-        <v>42924</v>
-      </c>
-      <c r="D21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="1">
-        <v>42924</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="1">
-        <v>42924</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1">
-        <v>42928</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="1">
-        <v>42924</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="1">
-        <v>42924</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
-        <v>42927</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="1">
-        <v>42928</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="2" t="s">
+      <c r="D32" t="s">
         <v>33</v>
-      </c>
-      <c r="C29" s="1">
-        <v>42928</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="1">
-        <v>42933</v>
-      </c>
-      <c r="D30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="1">
-        <v>42933</v>
-      </c>
-      <c r="D31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="1">
-        <v>42933</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C33" s="1">
-        <v>42933</v>
+        <v>42924</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1">
-        <v>42935</v>
+        <v>42903</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1">
-        <v>42935</v>
+        <v>42933</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1">
-        <v>42935</v>
+        <v>42933</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="E36" s="1">
+        <v>42942</v>
+      </c>
+      <c r="F36" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1">
-        <v>42935</v>
+        <v>42938</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="E37" s="1">
+        <v>42942</v>
+      </c>
+      <c r="F37" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1">
-        <v>42935</v>
+        <v>42940</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="E38" s="1">
+        <v>42942</v>
+      </c>
+      <c r="F38" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>42935</v>
+        <v>42903</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="E39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1">
-        <v>42938</v>
-      </c>
-      <c r="D40" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" t="s">
-        <v>51</v>
+        <v>42903</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C41" s="1">
-        <v>42938</v>
-      </c>
-      <c r="D41" t="s">
-        <v>52</v>
+        <v>42903</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="C42" s="1">
-        <v>42938</v>
-      </c>
-      <c r="D42" t="s">
-        <v>37</v>
+        <v>42903</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C43" s="1">
-        <v>42940</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
+        <v>42903</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C44" s="1">
-        <v>42940</v>
-      </c>
-      <c r="D44" t="s">
-        <v>11</v>
+        <v>42904</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C45" s="1">
-        <v>42940</v>
-      </c>
-      <c r="D45" t="s">
-        <v>11</v>
+        <v>42924</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C46" s="1">
-        <v>42940</v>
-      </c>
-      <c r="D46" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" t="s">
-        <v>58</v>
-      </c>
-      <c r="F46" t="s">
-        <v>11</v>
+        <v>42924</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="C47" s="1">
-        <v>42940</v>
-      </c>
-      <c r="D47" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" t="s">
-        <v>59</v>
+        <v>42933</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C48" s="1">
-        <v>42941</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+        <v>42933</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C49" s="1">
         <v>42941</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C50" s="1">
         <v>42941</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="C51" s="1">
+        <v>42941</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1">
+        <v>42942</v>
+      </c>
+      <c r="F51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="1">
+        <v>42941</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:D26">
-    <sortCondition ref="C2:C26"/>
+  <sortState ref="B1:F51">
+    <sortCondition ref="D2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated pause and end game screens
</commit_message>
<xml_diff>
--- a/TODO Spreadsheet.xlsx
+++ b/TODO Spreadsheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
   <si>
     <t>Transfer DODO txt document to Excel sheet</t>
   </si>
@@ -220,6 +220,33 @@
   </si>
   <si>
     <t>Don't need anymore</t>
+  </si>
+  <si>
+    <t>Pause Menu: Use screen interface</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Pause Menu: fix the green screen rendering after hitting resume</t>
+  </si>
+  <si>
+    <t>EndGameMenu: Make background not ugly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in progress </t>
+  </si>
+  <si>
+    <t>Make a shiny rainbow background?</t>
+  </si>
+  <si>
+    <t>TitleScreen: fix disappearing skybox/menu buttons glitch</t>
+  </si>
+  <si>
+    <t>Fix end game ranks based on armour/health if retire for timed game</t>
   </si>
 </sst>
 </file>
@@ -584,11 +611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,6 +1317,67 @@
       </c>
       <c r="C52" s="1">
         <v>42941</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="1">
+        <v>42947</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="1">
+        <v>42944</v>
+      </c>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="1">
+        <v>42947</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="1">
+        <v>42947</v>
+      </c>
+      <c r="D54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="1">
+        <v>42947</v>
+      </c>
+      <c r="D55" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="1">
+        <v>42947</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="1">
+        <v>42947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>